<commit_message>
Correction of attendance.ty file in delete option 3
There was an error when trying to delete a record
</commit_message>
<xml_diff>
--- a/student_attendance.xlsx
+++ b/student_attendance.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,160 +436,25 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Student</t>
+          <t>nen</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Course</t>
+          <t>ti</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Date</t>
+          <t>24/10/2025</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Time</t>
+          <t>17:29</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>nen</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>ti</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>22/10/2025</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>10:58</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Present</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>francisco_jose</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>ti</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>22/10/2025</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>10:59</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Present</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>nen</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>ingles</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>22/10/2025</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>10:59</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Absent</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>juju_pa</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>ti</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>22/10/2025</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>10:59</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Present</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>nen</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>ingles</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>22/10/2025</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>15:37</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
         <is>
           <t>Present</t>
         </is>

</xml_diff>